<commit_message>
started with functionality testing
</commit_message>
<xml_diff>
--- a/FB LoginPage TCs.xlsx
+++ b/FB LoginPage TCs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SQA\FBLoginTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF9F05D-951C-480A-B6BA-A6D0471E92E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EF9968-0DCC-4896-91AD-ED497F754F0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">TEST CASES ON FACEBOOK OF LOGIN PAGE </t>
   </si>
@@ -123,6 +123,45 @@
   <si>
     <t>Verify that the login functionality should work in different
 browsers. (Cross browser testing).</t>
+  </si>
+  <si>
+    <t>Verify that placeholder and tooltip are present or not.</t>
+  </si>
+  <si>
+    <t>TC-012</t>
+  </si>
+  <si>
+    <t>TC-013</t>
+  </si>
+  <si>
+    <t>Verify that the login screen is responsive according to different screen sizes. (Responsive Testing).</t>
+  </si>
+  <si>
+    <t>TC-014</t>
+  </si>
+  <si>
+    <t>TC-015</t>
+  </si>
+  <si>
+    <t>Verify that user is able to input username and password.</t>
+  </si>
+  <si>
+    <t>Verify that password is masked/encrypted.</t>
+  </si>
+  <si>
+    <t>Verify that password should be visible when eye button is clicked and vice-versa.</t>
+  </si>
+  <si>
+    <t>TC-016</t>
+  </si>
+  <si>
+    <t>TC-017</t>
+  </si>
+  <si>
+    <t>TC-018</t>
+  </si>
+  <si>
+    <t>TC-019</t>
   </si>
 </sst>
 </file>
@@ -520,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +764,61 @@
         <v>31</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I2"/>

</xml_diff>